<commit_message>
some news - work for big update
</commit_message>
<xml_diff>
--- a/datas/DataSet.xlsx
+++ b/datas/DataSet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matvey/PycharmProjects/Automatic-TAS/datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831AD896-D390-9648-99BC-5F0AF12E8ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920E2ED7-F8D4-D44B-8B04-D18575586E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Входные данные для анализа" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>№ точки</t>
   </si>
@@ -54,9 +54,6 @@
     <t>нет</t>
   </si>
   <si>
-    <t>ул. им. Максима Горького, д. 128</t>
-  </si>
-  <si>
     <t>давно</t>
   </si>
   <si>
@@ -352,6 +349,15 @@
   </si>
   <si>
     <t>ab5b44c446644ce7ec24ffd58a16233d9a8c887cfe8832b280a644abd91cbaab</t>
+  </si>
+  <si>
+    <t>ул. им. Дзержинского, д. 101</t>
+  </si>
+  <si>
+    <t>ул. им. Дзержинского, д. 102</t>
+  </si>
+  <si>
+    <t>ул. Горького, д. 128</t>
   </si>
 </sst>
 </file>
@@ -717,9 +723,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -772,13 +783,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -795,13 +806,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -818,13 +829,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -841,10 +852,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -864,13 +875,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>12</v>
@@ -887,13 +898,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>27</v>
@@ -910,13 +921,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>33</v>
@@ -933,13 +944,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -956,13 +967,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -979,13 +990,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>15</v>
@@ -1002,7 +1013,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1025,13 +1036,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1048,7 +1059,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1071,13 +1082,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>7</v>
@@ -1094,7 +1105,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1117,7 +1128,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1125,7 +1136,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1133,13 +1144,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -1156,13 +1167,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21">
         <v>4</v>
@@ -1179,7 +1190,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -1202,13 +1213,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -1225,13 +1236,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1248,13 +1259,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1271,7 +1282,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -1294,13 +1305,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1317,13 +1328,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1340,13 +1351,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1363,13 +1374,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E30">
         <v>6</v>
@@ -1386,13 +1397,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>16</v>
@@ -1409,13 +1420,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1432,13 +1443,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1455,7 +1466,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -1478,13 +1489,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E35">
         <v>76</v>
@@ -1501,13 +1512,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>23</v>
@@ -1524,13 +1535,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -1547,13 +1558,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E38">
         <v>9</v>
@@ -1570,7 +1581,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -1593,7 +1604,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
@@ -1616,13 +1627,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -1639,13 +1650,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -1662,13 +1673,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -1685,7 +1696,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -1718,25 +1729,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1744,22 +1755,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1767,22 +1778,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>66</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>67</v>
-      </c>
-      <c r="G3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1790,22 +1801,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1825,155 +1836,155 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
         <v>85</v>
       </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>86</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
         <v>89</v>
       </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>91</v>
-      </c>
-      <c r="E4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
         <v>93</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
         <v>94</v>
       </c>
-      <c r="C5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
         <v>100</v>
       </c>
-      <c r="B7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>101</v>
-      </c>
-      <c r="E7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
         <v>103</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
         <v>104</v>
       </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>105</v>
-      </c>
-      <c r="E8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
         <v>107</v>
       </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>108</v>
-      </c>
-      <c r="E9" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>